<commit_message>
added preparer column for hakon
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zirconion\Documents\GitHub\Splatnet3-img-stat-grab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zirconion\Documents\GitHub\Splatnet3-img-stat-grab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F12AE-28AB-44F2-AE1E-73C42F27D257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36102447-2293-4BD3-8475-83FB00E9BFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Map</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Team 2 (Loser)</t>
+  </si>
+  <si>
+    <t>Preparer</t>
   </si>
 </sst>
 </file>
@@ -542,224 +545,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK1"/>
+  <dimension ref="A1:BL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="BL1" sqref="BL1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>41</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>49</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>